<commit_message>
Updated to match accepted publication
Added some quantitative summaries and re-numbered figures to match accepted version.  Readme updated to match.
</commit_message>
<xml_diff>
--- a/Figures/RefftANOVAtable.xlsx
+++ b/Figures/RefftANOVAtable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wchiu/Dropbox/WCHIU-Documents/COVID-19-Bayesian-SEIR-US/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82379F59-FA33-474C-BCA1-4FFB12C67ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ACDBC4-0B49-3448-A931-1410E00D3FA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BFD51C5D-B2F8-2940-AEF1-DFA3F9A9140C}"/>
+    <workbookView xWindow="10420" yWindow="2460" windowWidth="28040" windowHeight="16320" xr2:uid="{BFD51C5D-B2F8-2940-AEF1-DFA3F9A9140C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Response:</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Df</t>
   </si>
   <si>
-    <t>Sum Sq</t>
-  </si>
-  <si>
-    <t>Mean Sq</t>
-  </si>
-  <si>
     <t>F value</t>
   </si>
   <si>
@@ -69,22 +63,22 @@
     <t>rho</t>
   </si>
   <si>
-    <t>Residuals</t>
-  </si>
-  <si>
     <t>rMax</t>
   </si>
   <si>
     <t>&lt; 2.2e-16</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Refft</t>
   </si>
   <si>
-    <t>Pct Sum Sq</t>
+    <t>lower CI</t>
+  </si>
+  <si>
+    <t>Upper CI</t>
+  </si>
+  <si>
+    <t>eta_sq</t>
   </si>
 </sst>
 </file>
@@ -131,10 +125,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E79AA3-7C82-6D48-8854-E06B40725C41}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -463,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -471,172 +466,166 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>72.400000000000006</v>
+      <c r="C3" s="2">
+        <v>6.2751162499999999E-2</v>
       </c>
       <c r="D3" s="2">
-        <f>C3/$C$12</f>
-        <v>6.2747545132298521E-2</v>
-      </c>
-      <c r="E3">
-        <v>72.403999999999996</v>
+        <v>5.7181309999999999E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.8523414099999999E-2</v>
       </c>
       <c r="F3">
         <v>3737.1329999999998</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>57.91</v>
+      <c r="C4" s="2">
+        <v>5.0191861900000002E-2</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D11" si="0">C4/$C$12</f>
-        <v>5.0189369317837115E-2</v>
-      </c>
-      <c r="E4">
-        <v>57.912999999999997</v>
-      </c>
-      <c r="F4">
+        <v>4.5146110000000003E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.5458764299999998E-2</v>
+      </c>
+      <c r="F4" s="3">
         <v>2989.1660000000002</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>100.31</v>
+      <c r="C5" s="2">
+        <v>8.6934278300000001E-2</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>8.6936550445039576E-2</v>
-      </c>
-      <c r="E5">
-        <v>100.30800000000001</v>
-      </c>
-      <c r="F5">
+        <v>8.0556619999999995E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.3480604499999995E-2</v>
+      </c>
+      <c r="F5" s="3">
         <v>5177.3540000000003</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>155.99</v>
+      <c r="C6" s="2">
+        <v>0.13519664679999999</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1351932260384979</v>
-      </c>
-      <c r="E6">
-        <v>155.995</v>
-      </c>
-      <c r="F6">
+        <v>0.12771440000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.14278621750000001</v>
+      </c>
+      <c r="F6" s="3">
         <v>8051.61</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>268.02999999999997</v>
+      <c r="C7" s="2">
+        <v>0.23229114009999999</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.23229591880952999</v>
-      </c>
-      <c r="E7">
-        <v>268.02600000000001</v>
-      </c>
-      <c r="F7">
+        <v>0.22375709999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.26862645610000002</v>
+      </c>
+      <c r="F7" s="3">
         <v>13834.053</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>0.41</v>
+      <c r="C8" s="2">
+        <v>3.5839429999999999E-4</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>3.5533830806964631E-4</v>
-      </c>
-      <c r="E8">
-        <v>0.41399999999999998</v>
+        <v>4.4311109999999997E-5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>9.7310769999999999E-4</v>
       </c>
       <c r="F8">
         <v>21.344000000000001</v>
@@ -645,25 +634,24 @@
         <v>3.8569999999999997E-6</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>0.91</v>
+      <c r="C9" s="2">
+        <v>7.8604629999999998E-4</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>7.8867770815458087E-4</v>
-      </c>
-      <c r="E9">
-        <v>0.90700000000000003</v>
+        <v>2.4864990000000002E-4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.62338E-3</v>
       </c>
       <c r="F9">
         <v>46.813000000000002</v>
@@ -672,61 +660,33 @@
         <v>7.9869999999999998E-12</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>4</v>
+      <c r="C10" s="2">
+        <v>3.4645367000000001E-3</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="0"/>
-        <v>3.4667152006794765E-3</v>
-      </c>
-      <c r="E10">
-        <v>3.9980000000000002</v>
+        <v>2.174011E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5.0504809999999999E-3</v>
       </c>
       <c r="F10">
         <v>206.33</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>25491</v>
-      </c>
-      <c r="C11">
-        <v>493.87</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.42802665903989323</v>
-      </c>
-      <c r="E11">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <f>SUM(C3:C11)</f>
-        <v>1153.83</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>